<commit_message>
Update Tables + Extra Generation for T/U/B/100
</commit_message>
<xml_diff>
--- a/TowerDefense/runs/tournament uniform bitstring 100/export.xlsx
+++ b/TowerDefense/runs/tournament uniform bitstring 100/export.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Users\Owner\Documents\GitHub\Y3-AoAIiG-EvolutionaryAlgorithms\TowerDefense\runs\tournament uniform bitstring 100\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C489AF03-9DDE-4E16-A306-A6B6EB14AFCB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE692A4A-5C35-4DB2-89A4-F9BD279FCA26}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="export" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -671,10 +671,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>export!$A$2:$A$9</c:f>
+              <c:f>export!$A$2:$A$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="8"/>
+                <c:ptCount val="9"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -698,16 +698,19 @@
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>8</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>export!$B$2:$B$9</c:f>
+              <c:f>export!$B$2:$B$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="8"/>
+                <c:ptCount val="9"/>
                 <c:pt idx="0">
                   <c:v>98</c:v>
                 </c:pt>
@@ -731,6 +734,9 @@
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>170</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>205</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -738,7 +744,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-F808-4DB8-B155-3EAE88AD3B82}"/>
+              <c16:uniqueId val="{00000000-6B49-4EA8-95F0-807899B93219}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -780,10 +786,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>export!$A$2:$A$9</c:f>
+              <c:f>export!$A$2:$A$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="8"/>
+                <c:ptCount val="9"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -807,16 +813,19 @@
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>8</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>export!$C$2:$C$9</c:f>
+              <c:f>export!$C$2:$C$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="8"/>
+                <c:ptCount val="9"/>
                 <c:pt idx="0">
                   <c:v>72</c:v>
                 </c:pt>
@@ -840,6 +849,9 @@
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>151</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>193</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -847,7 +859,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-F808-4DB8-B155-3EAE88AD3B82}"/>
+              <c16:uniqueId val="{00000001-6B49-4EA8-95F0-807899B93219}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -889,10 +901,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>export!$A$2:$A$9</c:f>
+              <c:f>export!$A$2:$A$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="8"/>
+                <c:ptCount val="9"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -916,16 +928,19 @@
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>8</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>export!$D$2:$D$9</c:f>
+              <c:f>export!$D$2:$D$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="8"/>
+                <c:ptCount val="9"/>
                 <c:pt idx="0">
                   <c:v>57</c:v>
                 </c:pt>
@@ -949,6 +964,9 @@
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>176</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>163</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -956,7 +974,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000002-F808-4DB8-B155-3EAE88AD3B82}"/>
+              <c16:uniqueId val="{00000002-6B49-4EA8-95F0-807899B93219}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -998,10 +1016,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>export!$A$2:$A$9</c:f>
+              <c:f>export!$A$2:$A$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="8"/>
+                <c:ptCount val="9"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -1025,16 +1043,19 @@
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>8</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>export!$E$2:$E$9</c:f>
+              <c:f>export!$E$2:$E$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="8"/>
+                <c:ptCount val="9"/>
                 <c:pt idx="0">
                   <c:v>51</c:v>
                 </c:pt>
@@ -1058,6 +1079,9 @@
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>143</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>198</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1065,7 +1089,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000003-F808-4DB8-B155-3EAE88AD3B82}"/>
+              <c16:uniqueId val="{00000003-6B49-4EA8-95F0-807899B93219}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1107,10 +1131,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>export!$A$2:$A$9</c:f>
+              <c:f>export!$A$2:$A$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="8"/>
+                <c:ptCount val="9"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -1134,16 +1158,19 @@
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>8</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>export!$F$2:$F$9</c:f>
+              <c:f>export!$F$2:$F$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="8"/>
+                <c:ptCount val="9"/>
                 <c:pt idx="0">
                   <c:v>50</c:v>
                 </c:pt>
@@ -1167,6 +1194,9 @@
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>195</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>194</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1174,7 +1204,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000004-F808-4DB8-B155-3EAE88AD3B82}"/>
+              <c16:uniqueId val="{00000004-6B49-4EA8-95F0-807899B93219}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1216,10 +1246,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>export!$A$2:$A$9</c:f>
+              <c:f>export!$A$2:$A$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="8"/>
+                <c:ptCount val="9"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -1243,16 +1273,19 @@
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>8</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>export!$G$2:$G$9</c:f>
+              <c:f>export!$G$2:$G$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="8"/>
+                <c:ptCount val="9"/>
                 <c:pt idx="0">
                   <c:v>43</c:v>
                 </c:pt>
@@ -1276,6 +1309,9 @@
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>175</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1283,7 +1319,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000005-F808-4DB8-B155-3EAE88AD3B82}"/>
+              <c16:uniqueId val="{00000005-6B49-4EA8-95F0-807899B93219}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1329,10 +1365,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>export!$A$2:$A$9</c:f>
+              <c:f>export!$A$2:$A$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="8"/>
+                <c:ptCount val="9"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -1356,16 +1392,19 @@
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>8</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>export!$H$2:$H$9</c:f>
+              <c:f>export!$H$2:$H$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="8"/>
+                <c:ptCount val="9"/>
                 <c:pt idx="0">
                   <c:v>40</c:v>
                 </c:pt>
@@ -1389,6 +1428,9 @@
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>130</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1396,7 +1438,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000006-F808-4DB8-B155-3EAE88AD3B82}"/>
+              <c16:uniqueId val="{00000006-6B49-4EA8-95F0-807899B93219}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1442,10 +1484,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>export!$A$2:$A$9</c:f>
+              <c:f>export!$A$2:$A$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="8"/>
+                <c:ptCount val="9"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -1469,16 +1511,19 @@
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>8</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>export!$I$2:$I$9</c:f>
+              <c:f>export!$I$2:$I$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="8"/>
+                <c:ptCount val="9"/>
                 <c:pt idx="0">
                   <c:v>40</c:v>
                 </c:pt>
@@ -1502,6 +1547,9 @@
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>176</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>151</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1509,7 +1557,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000007-F808-4DB8-B155-3EAE88AD3B82}"/>
+              <c16:uniqueId val="{00000007-6B49-4EA8-95F0-807899B93219}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1528,7 +1576,7 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="25400" cap="rnd">
+            <a:ln w="19050" cap="rnd">
               <a:noFill/>
               <a:round/>
             </a:ln>
@@ -1555,10 +1603,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>export!$A$2:$A$9</c:f>
+              <c:f>export!$A$2:$A$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="8"/>
+                <c:ptCount val="9"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -1582,16 +1630,19 @@
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>8</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>export!$J$2:$J$9</c:f>
+              <c:f>export!$J$2:$J$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="8"/>
+                <c:ptCount val="9"/>
                 <c:pt idx="0">
                   <c:v>69</c:v>
                 </c:pt>
@@ -1615,6 +1666,9 @@
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>195</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>143</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1622,7 +1676,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000008-F808-4DB8-B155-3EAE88AD3B82}"/>
+              <c16:uniqueId val="{00000008-6B49-4EA8-95F0-807899B93219}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1641,7 +1695,7 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="25400" cap="rnd">
+            <a:ln w="19050" cap="rnd">
               <a:noFill/>
               <a:round/>
             </a:ln>
@@ -1668,10 +1722,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>export!$A$2:$A$9</c:f>
+              <c:f>export!$A$2:$A$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="8"/>
+                <c:ptCount val="9"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -1695,16 +1749,19 @@
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>8</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>export!$K$2:$K$9</c:f>
+              <c:f>export!$K$2:$K$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="8"/>
+                <c:ptCount val="9"/>
                 <c:pt idx="0">
                   <c:v>50</c:v>
                 </c:pt>
@@ -1728,6 +1785,9 @@
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>170</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>175</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1735,7 +1795,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000009-F808-4DB8-B155-3EAE88AD3B82}"/>
+              <c16:uniqueId val="{00000009-6B49-4EA8-95F0-807899B93219}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1754,7 +1814,7 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="25400" cap="rnd">
+            <a:ln w="19050" cap="rnd">
               <a:noFill/>
               <a:round/>
             </a:ln>
@@ -1781,10 +1841,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>export!$A$2:$A$9</c:f>
+              <c:f>export!$A$2:$A$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="8"/>
+                <c:ptCount val="9"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -1808,16 +1868,19 @@
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>8</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>export!$L$2:$L$9</c:f>
+              <c:f>export!$L$2:$L$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="8"/>
+                <c:ptCount val="9"/>
                 <c:pt idx="0">
                   <c:v>151</c:v>
                 </c:pt>
@@ -1841,6 +1904,9 @@
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>170</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>162</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1848,7 +1914,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{0000000A-F808-4DB8-B155-3EAE88AD3B82}"/>
+              <c16:uniqueId val="{0000000A-6B49-4EA8-95F0-807899B93219}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1867,7 +1933,7 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="25400" cap="rnd">
+            <a:ln w="19050" cap="rnd">
               <a:noFill/>
               <a:round/>
             </a:ln>
@@ -1894,10 +1960,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>export!$A$2:$A$9</c:f>
+              <c:f>export!$A$2:$A$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="8"/>
+                <c:ptCount val="9"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -1921,16 +1987,19 @@
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>8</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>export!$M$2:$M$9</c:f>
+              <c:f>export!$M$2:$M$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="8"/>
+                <c:ptCount val="9"/>
                 <c:pt idx="0">
                   <c:v>83</c:v>
                 </c:pt>
@@ -1954,6 +2023,9 @@
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>152</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>171</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1961,7 +2033,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{0000000B-F808-4DB8-B155-3EAE88AD3B82}"/>
+              <c16:uniqueId val="{0000000B-6B49-4EA8-95F0-807899B93219}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1980,7 +2052,7 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="25400" cap="rnd">
+            <a:ln w="19050" cap="rnd">
               <a:noFill/>
               <a:round/>
             </a:ln>
@@ -2009,10 +2081,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>export!$A$2:$A$9</c:f>
+              <c:f>export!$A$2:$A$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="8"/>
+                <c:ptCount val="9"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -2036,16 +2108,19 @@
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>8</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>export!$N$2:$N$9</c:f>
+              <c:f>export!$N$2:$N$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="8"/>
+                <c:ptCount val="9"/>
                 <c:pt idx="0">
                   <c:v>69</c:v>
                 </c:pt>
@@ -2069,6 +2144,9 @@
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>150</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>144</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2076,7 +2154,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{0000000C-F808-4DB8-B155-3EAE88AD3B82}"/>
+              <c16:uniqueId val="{0000000C-6B49-4EA8-95F0-807899B93219}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -2095,7 +2173,7 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="25400" cap="rnd">
+            <a:ln w="19050" cap="rnd">
               <a:noFill/>
               <a:round/>
             </a:ln>
@@ -2124,10 +2202,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>export!$A$2:$A$9</c:f>
+              <c:f>export!$A$2:$A$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="8"/>
+                <c:ptCount val="9"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -2151,16 +2229,19 @@
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>8</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>export!$O$2:$O$9</c:f>
+              <c:f>export!$O$2:$O$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="8"/>
+                <c:ptCount val="9"/>
                 <c:pt idx="0">
                   <c:v>45</c:v>
                 </c:pt>
@@ -2184,6 +2265,9 @@
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>125</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>193</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2191,7 +2275,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{0000000D-F808-4DB8-B155-3EAE88AD3B82}"/>
+              <c16:uniqueId val="{0000000D-6B49-4EA8-95F0-807899B93219}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -2210,7 +2294,7 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="25400" cap="rnd">
+            <a:ln w="19050" cap="rnd">
               <a:noFill/>
               <a:round/>
             </a:ln>
@@ -2239,10 +2323,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>export!$A$2:$A$9</c:f>
+              <c:f>export!$A$2:$A$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="8"/>
+                <c:ptCount val="9"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -2266,16 +2350,19 @@
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>8</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>export!$P$2:$P$9</c:f>
+              <c:f>export!$P$2:$P$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="8"/>
+                <c:ptCount val="9"/>
                 <c:pt idx="0">
                   <c:v>57</c:v>
                 </c:pt>
@@ -2299,6 +2386,9 @@
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>114</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>105</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2306,7 +2396,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{0000000E-F808-4DB8-B155-3EAE88AD3B82}"/>
+              <c16:uniqueId val="{0000000E-6B49-4EA8-95F0-807899B93219}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -2325,7 +2415,7 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="25400" cap="rnd">
+            <a:ln w="19050" cap="rnd">
               <a:noFill/>
               <a:round/>
             </a:ln>
@@ -2354,10 +2444,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>export!$A$2:$A$9</c:f>
+              <c:f>export!$A$2:$A$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="8"/>
+                <c:ptCount val="9"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -2381,16 +2471,19 @@
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>8</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>export!$Q$2:$Q$9</c:f>
+              <c:f>export!$Q$2:$Q$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="8"/>
+                <c:ptCount val="9"/>
                 <c:pt idx="0">
                   <c:v>94</c:v>
                 </c:pt>
@@ -2414,6 +2507,9 @@
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>169</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>166</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2421,7 +2517,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{0000000F-F808-4DB8-B155-3EAE88AD3B82}"/>
+              <c16:uniqueId val="{0000000F-6B49-4EA8-95F0-807899B93219}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -2433,13 +2529,14 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="1197808607"/>
-        <c:axId val="1274692895"/>
+        <c:axId val="843847712"/>
+        <c:axId val="714767920"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="1197808607"/>
+        <c:axId val="843847712"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="8"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
@@ -2549,15 +2646,15 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1274692895"/>
+        <c:crossAx val="714767920"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1274692895"/>
+        <c:axId val="714767920"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="200"/>
+          <c:max val="220"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -2667,9 +2764,10 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1197808607"/>
+        <c:crossAx val="843847712"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
+        <c:majorUnit val="20"/>
       </c:valAx>
       <c:spPr>
         <a:noFill/>
@@ -3316,25 +3414,27 @@
     <xdr:from>
       <xdr:col>18</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>4761</xdr:rowOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>190499</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>24</xdr:col>
-      <xdr:colOff>609599</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>185738</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1">
+        <xdr:cNvPr id="3" name="Chart 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0BE7C845-044A-E1D1-66D2-F2BFBE23AEBD}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DDEA8E9C-F4CA-4B65-AB53-4265A30D11E3}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
-        <xdr:cNvGraphicFramePr/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="0" y="0"/>
@@ -3647,11 +3747,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q9"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:Q10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="V20" sqref="V20"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="S2" sqref="S2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4130,6 +4230,59 @@
         <v>169</v>
       </c>
     </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>8</v>
+      </c>
+      <c r="B10">
+        <v>205</v>
+      </c>
+      <c r="C10">
+        <v>193</v>
+      </c>
+      <c r="D10">
+        <v>163</v>
+      </c>
+      <c r="E10">
+        <v>198</v>
+      </c>
+      <c r="F10">
+        <v>194</v>
+      </c>
+      <c r="G10">
+        <v>175</v>
+      </c>
+      <c r="H10">
+        <v>130</v>
+      </c>
+      <c r="I10">
+        <v>151</v>
+      </c>
+      <c r="J10">
+        <v>143</v>
+      </c>
+      <c r="K10">
+        <v>175</v>
+      </c>
+      <c r="L10">
+        <v>162</v>
+      </c>
+      <c r="M10">
+        <v>171</v>
+      </c>
+      <c r="N10">
+        <v>144</v>
+      </c>
+      <c r="O10">
+        <v>193</v>
+      </c>
+      <c r="P10">
+        <v>105</v>
+      </c>
+      <c r="Q10">
+        <v>166</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>